<commit_message>
Refactor inferensi and defuzzifikasi functions to clarify rule application and update documentation for 9 rules.
</commit_message>
<xml_diff>
--- a/peringkat.xlsx
+++ b/peringkat.xlsx
@@ -445,13 +445,13 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>22</v>
+        <v>79</v>
       </c>
       <c r="B2" t="n">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="C2" t="n">
-        <v>39211</v>
+        <v>22360</v>
       </c>
       <c r="D2" t="n">
         <v>90</v>
@@ -459,128 +459,128 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>25</v>
+        <v>80</v>
       </c>
       <c r="B3" t="n">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C3" t="n">
-        <v>34513</v>
+        <v>22012</v>
       </c>
       <c r="D3" t="n">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="B4" t="n">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C4" t="n">
-        <v>38869</v>
+        <v>27315</v>
       </c>
       <c r="D4" t="n">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="B5" t="n">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="C5" t="n">
-        <v>22360</v>
+        <v>24551</v>
       </c>
       <c r="D5" t="n">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B6" t="n">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="C6" t="n">
-        <v>35304</v>
+        <v>29811</v>
       </c>
       <c r="D6" t="n">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>80</v>
+        <v>25</v>
       </c>
       <c r="B7" t="n">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="C7" t="n">
-        <v>22012</v>
+        <v>34513</v>
       </c>
       <c r="D7" t="n">
-        <v>89.5</v>
+        <v>80.97399999999999</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="B8" t="n">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C8" t="n">
-        <v>27315</v>
+        <v>20052</v>
       </c>
       <c r="D8" t="n">
-        <v>88</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>69</v>
+        <v>88</v>
       </c>
       <c r="B9" t="n">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="C9" t="n">
-        <v>24551</v>
+        <v>35304</v>
       </c>
       <c r="D9" t="n">
-        <v>87.5</v>
+        <v>79.392</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>86</v>
+        <v>23</v>
       </c>
       <c r="B10" t="n">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C10" t="n">
-        <v>29811</v>
+        <v>22825</v>
       </c>
       <c r="D10" t="n">
-        <v>87</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>66</v>
+        <v>33</v>
       </c>
       <c r="B11" t="n">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="C11" t="n">
-        <v>20052</v>
+        <v>24704</v>
       </c>
       <c r="D11" t="n">
-        <v>85</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update defuzzification weights for improved ranking accuracy and modify peringkat.xlsx with new data
</commit_message>
<xml_diff>
--- a/peringkat.xlsx
+++ b/peringkat.xlsx
@@ -454,7 +454,7 @@
         <v>22360</v>
       </c>
       <c r="D2" t="n">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3">
@@ -468,7 +468,7 @@
         <v>22012</v>
       </c>
       <c r="D3" t="n">
-        <v>89</v>
+        <v>98.75</v>
       </c>
     </row>
     <row r="4">
@@ -482,7 +482,7 @@
         <v>27315</v>
       </c>
       <c r="D4" t="n">
-        <v>86</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5">
@@ -496,7 +496,7 @@
         <v>24551</v>
       </c>
       <c r="D5" t="n">
-        <v>85</v>
+        <v>93.75</v>
       </c>
     </row>
     <row r="6">
@@ -510,7 +510,7 @@
         <v>29811</v>
       </c>
       <c r="D6" t="n">
-        <v>84</v>
+        <v>92.5</v>
       </c>
     </row>
     <row r="7">
@@ -524,7 +524,7 @@
         <v>34513</v>
       </c>
       <c r="D7" t="n">
-        <v>80.97399999999999</v>
+        <v>88.7175</v>
       </c>
     </row>
     <row r="8">
@@ -538,7 +538,7 @@
         <v>20052</v>
       </c>
       <c r="D8" t="n">
-        <v>80</v>
+        <v>87.5</v>
       </c>
     </row>
     <row r="9">
@@ -552,7 +552,7 @@
         <v>35304</v>
       </c>
       <c r="D9" t="n">
-        <v>79.392</v>
+        <v>86.74000000000001</v>
       </c>
     </row>
     <row r="10">
@@ -566,7 +566,7 @@
         <v>22825</v>
       </c>
       <c r="D10" t="n">
-        <v>77</v>
+        <v>83.75</v>
       </c>
     </row>
     <row r="11">
@@ -580,7 +580,7 @@
         <v>24704</v>
       </c>
       <c r="D11" t="n">
-        <v>73</v>
+        <v>78.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>